<commit_message>
Kalia Network - Adding Stage 3 Evidence for B1-B2
</commit_message>
<xml_diff>
--- a/KaliaNetwork/evidence.xlsx
+++ b/KaliaNetwork/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_KaliaNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE33936-15F0-401A-BD47-6D6F7C91243F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE49377-0439-4295-897A-01FAECCC2519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="842" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="53">
   <si>
     <t>TxHash</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>8582434B711A8F87259101B197F9F2BD35B45707C7042E1D794EE8D05FA7EC83</t>
+  </si>
+  <si>
+    <t>EBA77C6A2D9A762D425858527CA17EB3AE88113A98E22F61CEC03C4361C55552</t>
+  </si>
+  <si>
+    <t>9F235F8868FAD3543DF8595F9C381FC49BF61723B3A7B9F0D6EFC773807FE003</t>
+  </si>
+  <si>
+    <t>F6A1B4FD53BAEC0088E51F9872C2AAF5EE732950928D0FF1861AB21EE73741C3</t>
+  </si>
+  <si>
+    <t>88BA16398AB92E3C2AD64D094AC9B1ADF266089507D8CDABBC9B1EB9C1899B17</t>
   </si>
 </sst>
 </file>
@@ -1262,6 +1274,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1289,8 +1373,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1323,74 +1407,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
@@ -1651,7 +1667,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Kalia Network - Adding Stage 2 Evidence for A7-A20
</commit_message>
<xml_diff>
--- a/KaliaNetwork/evidence.xlsx
+++ b/KaliaNetwork/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0K_KaliaNetwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0K_KaliaNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE49377-0439-4295-897A-01FAECCC2519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1C04D1-AD41-443F-A033-D80B108FCF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="842" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="842" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -203,13 +188,166 @@
   </si>
   <si>
     <t>88BA16398AB92E3C2AD64D094AC9B1ADF266089507D8CDABBC9B1EB9C1899B17</t>
+  </si>
+  <si>
+    <t>ibc/D873C033B41683EF36B74EB44001EF7C1C5674D935178560921F49E3CF40A443</t>
+  </si>
+  <si>
+    <t>kalianetworka7</t>
+  </si>
+  <si>
+    <t>ibc/34D46AD2667D638B8B566E368E4B686A793D165B12F634A620F621BE494B14DE</t>
+  </si>
+  <si>
+    <t>kalianetworka8</t>
+  </si>
+  <si>
+    <t>kalianetworka9</t>
+  </si>
+  <si>
+    <t>ibc/D1677F9B178BDB98ADF4237A4ADC06410440C6F2EA045831A61594CF89F988B9</t>
+  </si>
+  <si>
+    <t>kalianetworka10</t>
+  </si>
+  <si>
+    <t>ibc/A23E035203B8C36FBF5D422C5AD5EDA3AFBB211F8D83BC297FA65D77C88FC96B</t>
+  </si>
+  <si>
+    <t>kalianetworka11</t>
+  </si>
+  <si>
+    <t>ibc/4C1CEFB89E34028D0B76419DC1A8812B39F476E3D7F604E2026342E0CDD7AAD9</t>
+  </si>
+  <si>
+    <t>kalianetworka12</t>
+  </si>
+  <si>
+    <t>ibc/7F99F91378A90215773C377DD2A4BE8C819F240C51CB353999F35F5E5A92C977</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>3B2EB0D5C207C8D4F1B81F7DC7C65D6ED577A9BD73C5F295C05710F782A77C15</t>
+  </si>
+  <si>
+    <t>22A59D0DD77D89DF45E4603087235651DCA3E2F9135DB9B75824578272EB388E</t>
+  </si>
+  <si>
+    <t>C14F0FCDEFFF3441737D76AF6C5D59DF8CD0F7C8E69A8016A55C6EE1618658A6</t>
+  </si>
+  <si>
+    <t>6F1FE0029304295972E431B92660104881DFB509B37520634D470879BFAF57EC</t>
+  </si>
+  <si>
+    <t>A5677652AFE80708271404FEF6E523981CC31A8B6444D09815218A665558530D</t>
+  </si>
+  <si>
+    <t>F40A501AD8249761CB884F29E54098B46256D747080FF22C7C42833650926D92</t>
+  </si>
+  <si>
+    <t>4501FDB2035BB9A7541BB6C404C5A05190F4B4DB8D2A03C076A933D595481FFB</t>
+  </si>
+  <si>
+    <t>E1C68088675F181B399FF957CF5ABD0AA85140B8B8F81E5E57BA1FD8F170E5CA</t>
+  </si>
+  <si>
+    <t>47FDD3C265E64EB6618DD465796034540AF95C9F8C3136FDCEA183C8C68C52E7</t>
+  </si>
+  <si>
+    <t>8E94E10E5FCC8AC6C524F697770CBE0A3F3A0615FA3BDFECD5D4F80441B7C04C</t>
+  </si>
+  <si>
+    <t>7B06A31D443E2B7EC8F30CAAEE6F9D5622EAA8E8D1037E1BFBCA402F591BDE70</t>
+  </si>
+  <si>
+    <t>22C280DA3D0AD4A1AEECB88D2B0AE3FE776CE34E604791EA2657A2BE4CBC8413</t>
+  </si>
+  <si>
+    <t>731B368FE8B14E4CCDFA2123C4984223E623BAA28EEECAC3C21D3621F1A8F1D2</t>
+  </si>
+  <si>
+    <t>20975571462A41FA2B70FFEC3BCE003DD565CB897B9876F5F8873F1E36DBC5E2</t>
+  </si>
+  <si>
+    <t>2BEFE3D5D44A86D6C85D5B3B8EBCEAFCC1BDEB77BC7CB57628F5B28935926396</t>
+  </si>
+  <si>
+    <t>D117A120CB806239AF4D3A105E0C084D40718BBC5D63384C75E9F380F34F2185</t>
+  </si>
+  <si>
+    <t>9A3AD74D9D88370491F46CA4FA5FC8AE216D913F08D0345587B75D346C8DF927</t>
+  </si>
+  <si>
+    <t>140B5AF6C03C8C21CAEAF81FAFAF229312B251CE378C8EB8C2286E2AAE725D8C</t>
+  </si>
+  <si>
+    <t>9C1D5591362FF5A98270519EB5E420EA801219E37E1E714BF0D86F6F29E9750D</t>
+  </si>
+  <si>
+    <t>CD3B68A7A1FE790063933938BF0E2FC5510240F04DC09376C6791CD85771250D</t>
+  </si>
+  <si>
+    <t>5116D562EFDC6C88B795262C05BBFA28BE42C729F4F8EE5FE228112C09798D15</t>
+  </si>
+  <si>
+    <t>B7A54B940680FA609C2C075FE51DCFD56DED4E442E16F56384C8326786843791</t>
+  </si>
+  <si>
+    <t>08A33BB99AED95737E21FD7FB3E857EA9E7FAD294C2E97437D65AC798C02C7F5</t>
+  </si>
+  <si>
+    <t>7A0BAFC95875E2AE54C04EDD3F25F1F2EA50FD3FE6ABC3829F5F50570491A562</t>
+  </si>
+  <si>
+    <t>5D63A20F1EC73ED5201A94535BD2D6D73748C5D0F2115D60376333929C01F620</t>
+  </si>
+  <si>
+    <t>90852B54ACB85C42DA8FC10C764EB9DC67EDCBB265261E45DC5967F74300BB85</t>
+  </si>
+  <si>
+    <t>C6532EF5D4932EFCD5BE2984D3E3662133B0BDC5BBF7D32AE3477E8606981DE0</t>
+  </si>
+  <si>
+    <t>E105D7D1201131AF849A6C60EAC846ACDE1D64413AE2E057AA6C34220C7A6538</t>
+  </si>
+  <si>
+    <t>2579230BCFF859AFB253611F72F7F54132E0F492AADFCB3B5E4F509469F84EE9</t>
+  </si>
+  <si>
+    <t>212CA7C848C6EBBB7D76FF68384C1C39844E64547CB2E61CC8942D366239BE7D</t>
+  </si>
+  <si>
+    <t>21F23700352504024BE0EC7BDE81AEA1465735597EBF7FC78E224D730000784E</t>
+  </si>
+  <si>
+    <t>10FF126B7AFE389518331A1746BB0F55FAB4282E4A03465192F17A94E3B998D5</t>
+  </si>
+  <si>
+    <t>BDCF4DDD442D208B7EEA2F6D6BF52F5E47E3DAE82287597E0AEC109F39F29004</t>
+  </si>
+  <si>
+    <t>C793B4F448EF471A2F65DD52141D57AD0F872B83643B758692500FCBB83B01CA</t>
+  </si>
+  <si>
+    <t>458E3948C574A88CAF32475A3936360CD14BD1BD06DA494F824C9A43209F9546</t>
+  </si>
+  <si>
+    <t>220E36D84B0B4CFC12B6E051F308AF45498A3FEC0F2C6CC3355BCEB273018CF1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +377,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -293,9 +437,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -305,7 +450,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -318,10 +462,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{56BEC423-8E9E-4A84-9916-5DB88806B7F0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -636,7 +784,7 @@
     <col min="2" max="2" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -644,54 +792,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +857,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -719,18 +869,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -745,7 +895,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -755,18 +907,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +933,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -791,18 +945,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +971,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -827,18 +983,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -851,9 +1007,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -871,25 +1029,38 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -899,9 +1070,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -919,23 +1092,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -947,9 +1132,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -967,23 +1154,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -995,9 +1194,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1015,23 +1216,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1043,9 +1256,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,23 +1278,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1091,9 +1318,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1111,23 +1340,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1155,15 +1396,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1176,9 +1417,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1196,23 +1439,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1224,9 +1495,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1244,23 +1517,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,12 +1591,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1611,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1326,12 +1627,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1429,76 +1730,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>45</v>
+      <c r="A7" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1530,10 +1831,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1541,16 +1842,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1581,10 +1882,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1592,16 +1893,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1632,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1643,16 +1944,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1684,10 +1985,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1695,16 +1996,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1719,7 +2020,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1729,18 +2032,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +2058,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1765,18 +2070,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kalia Network - Adding Round 4 Evidence for B5-B7
</commit_message>
<xml_diff>
--- a/KaliaNetwork/evidence.xlsx
+++ b/KaliaNetwork/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0K_KaliaNetwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_ALL_KaliaNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1C04D1-AD41-443F-A033-D80B108FCF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90AAC6B-0A16-4AAC-8C14-B5142040F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="842" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="842" firstSheet="5" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="103">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -341,6 +336,24 @@
   </si>
   <si>
     <t>220E36D84B0B4CFC12B6E051F308AF45498A3FEC0F2C6CC3355BCEB273018CF1</t>
+  </si>
+  <si>
+    <t>CFD997153B60111CE7A08C57F7B5BB2059B7112F66AB6813DF087F20B78B2CD8</t>
+  </si>
+  <si>
+    <t>05E5A2443511282C69FFC1CC5F519DD449EA2678D2062819EEEBA6B8E5B98363</t>
+  </si>
+  <si>
+    <t>F60E4243BAC017BBF43E1D541E5AD3B0A573A7CBF3AD0DDF1CD9DC61C32AF732</t>
+  </si>
+  <si>
+    <t>17C578979958CA31043F4792D1DF625F2D50EB11008E59BD0EDFC850FAE7C07A</t>
+  </si>
+  <si>
+    <t>0337AA14B1B142D2D0484897EFC56E0559D3146F04E7A6BECC437A4A780F9263</t>
+  </si>
+  <si>
+    <t>9D1CA29D64976998595833A18EDD997AD81CB98ADFE751C987A03F516EB165F8</t>
   </si>
 </sst>
 </file>
@@ -792,54 +805,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +882,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,8 +939,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -907,10 +958,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,15 +977,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,10 +996,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -964,15 +1015,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,27 +1034,52 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1024,49 +1100,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1087,55 +1162,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,55 +1224,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,48 +1286,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1273,55 +1348,92 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,92 +1447,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,133 +1525,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>91</v>
+      <c r="A6" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1590,6 +1603,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -1604,15 +1653,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,27 +1676,29 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1661,27 +1712,26 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E240CFD5-29EF-4B7D-BEA5-C21400E2B45A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1695,12 +1745,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1730,76 +1780,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1831,27 +1881,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1882,27 +1932,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1933,27 +1983,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1985,27 +2035,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2032,10 +2082,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,42 +2137,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>